<commit_message>
Adds an incomprehensible R script for generating growth curves from OD data, and attendant files.
</commit_message>
<xml_diff>
--- a/Drafts/Scraps/Nash_isolates.xlsx
+++ b/Drafts/Scraps/Nash_isolates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Welch\Google Drive\ICL Ecological Applications\Project\Work\Drafts\Scraps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6499F7B4-B77C-4133-B32F-DD5EC16FA2F6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC37E78E-E7F6-490A-AF64-30AFCCF26B27}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -9402,8 +9402,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T845"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N820" sqref="N820"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R429" sqref="R429:R441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -56602,8 +56602,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>